<commit_message>
popravlen ahl seznam z stetjem procentov
</commit_message>
<xml_diff>
--- a/data/ICEHLdelegacije.xlsx
+++ b/data/ICEHLdelegacije.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBDBAFF-D120-4EF6-8A6D-4662B7045840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="ICEHL" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="ICEHL_DAT" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="ICEHL_DAT_STRING" state="visible" r:id="rId6"/>
+    <sheet name="ICEHL" sheetId="1" r:id="rId1"/>
+    <sheet name="ICEHL_DAT" sheetId="3" r:id="rId2"/>
+    <sheet name="ICEHL_DAT_STRING" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="111">
   <si>
     <t>BernekerTh</t>
   </si>
@@ -159,12 +160,6 @@
     <t>ZacherlPa</t>
   </si>
   <si>
-    <t>2024-09-11</t>
-  </si>
-  <si>
-    <t>2024-09-15</t>
-  </si>
-  <si>
     <t>2024-09-20</t>
   </si>
   <si>
@@ -205,12 +200,6 @@
   </si>
   <si>
     <t>2024-10-11</t>
-  </si>
-  <si>
-    <t>Tiroler Wasserkraft Arena;BernekerTh;HuberAn;MartinFl;SparerDa</t>
-  </si>
-  <si>
-    <t>Stadthalle Villach;OfnerCh;SternatCh;BärnthalerCh;PuffWo</t>
   </si>
   <si>
     <t>Heidi Horten Arena Klagenfurt;GroznikBo;SternatCh;JedlickaPe;KoncDa</t>
@@ -366,28 +355,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -402,9 +385,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,14 +666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AV134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:AU134"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -750,7 +732,7 @@
     <col min="58" max="58" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -893,7 +875,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -904,284 +886,284 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" t="s">
+        <v>47</v>
+      </c>
+      <c r="X4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="AA4" t="s">
         <v>49</v>
       </c>
-      <c r="J4" t="s">
+      <c r="AB4" t="s">
         <v>49</v>
       </c>
-      <c r="K4" t="s">
+      <c r="AC4" t="s">
         <v>49</v>
       </c>
-      <c r="L4" t="s">
+      <c r="AD4" t="s">
         <v>49</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AE4" t="s">
         <v>49</v>
       </c>
-      <c r="N4" t="s">
+      <c r="AF4" t="s">
         <v>49</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AG4" t="s">
         <v>49</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AH4" t="s">
         <v>49</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AI4" t="s">
         <v>49</v>
       </c>
-      <c r="R4" t="s">
+      <c r="AJ4" t="s">
         <v>49</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AK4" t="s">
         <v>49</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AL4" t="s">
         <v>49</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AM4" t="s">
         <v>49</v>
       </c>
-      <c r="V4" t="s">
-        <v>49</v>
-      </c>
-      <c r="W4" t="s">
-        <v>49</v>
-      </c>
-      <c r="X4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AN4" t="s">
         <v>50</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AO4" t="s">
         <v>51</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AP4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="AC4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AT4" t="s">
+      <c r="B5" t="s">
         <v>57</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
       <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" t="s">
         <v>51</v>
       </c>
-      <c r="J5" t="s">
+      <c r="S5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T5" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" t="s">
+        <v>51</v>
+      </c>
+      <c r="V5" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" t="s">
         <v>53</v>
       </c>
-      <c r="K5" t="s">
+      <c r="Y5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA5" t="s">
         <v>53</v>
       </c>
-      <c r="L5" t="s">
+      <c r="AB5" t="s">
         <v>53</v>
       </c>
-      <c r="M5" t="s">
+      <c r="AC5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN5" t="s">
         <v>53</v>
       </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="AO5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR5" t="s">
         <v>55</v>
       </c>
-      <c r="P5" t="s">
+    </row>
+    <row r="6" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
         <v>51</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" t="s">
-        <v>53</v>
-      </c>
-      <c r="S5" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W5" t="s">
-        <v>53</v>
-      </c>
-      <c r="X5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
@@ -1190,114 +1172,111 @@
         <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" t="s">
+        <v>53</v>
+      </c>
+      <c r="S6" t="s">
+        <v>54</v>
+      </c>
+      <c r="T6" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" t="s">
+        <v>53</v>
+      </c>
+      <c r="W6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC6" t="s">
         <v>56</v>
       </c>
-      <c r="K6" t="s">
+      <c r="AD6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>60</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" t="s">
-        <v>54</v>
-      </c>
-      <c r="P6" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>55</v>
-      </c>
-      <c r="R6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S6" t="s">
-        <v>56</v>
-      </c>
-      <c r="T6" t="s">
-        <v>53</v>
-      </c>
-      <c r="U6" t="s">
-        <v>56</v>
-      </c>
-      <c r="V6" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6" t="s">
-        <v>55</v>
-      </c>
-      <c r="X6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -1306,246 +1285,225 @@
         <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
         <v>53</v>
       </c>
       <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
         <v>60</v>
       </c>
-      <c r="J7" t="s">
-        <v>62</v>
-      </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" t="s">
+        <v>54</v>
+      </c>
+      <c r="X7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" t="s">
+        <v>54</v>
+      </c>
+      <c r="U8" t="s">
+        <v>60</v>
+      </c>
+      <c r="W8" t="s">
+        <v>56</v>
+      </c>
+      <c r="X8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
         <v>59</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9" t="s">
         <v>56</v>
       </c>
-      <c r="N7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" t="s">
-        <v>62</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="T9" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Y9" t="s">
         <v>60</v>
       </c>
-      <c r="R7" t="s">
+    </row>
+    <row r="10" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>51</v>
+      </c>
+      <c r="T10" t="s">
         <v>60</v>
       </c>
-      <c r="S7" t="s">
-        <v>60</v>
-      </c>
-      <c r="T7" t="s">
-        <v>55</v>
-      </c>
-      <c r="U7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" t="s">
-        <v>57</v>
-      </c>
-      <c r="W7" t="s">
-        <v>56</v>
-      </c>
-      <c r="X7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" t="s">
-        <v>58</v>
-      </c>
-      <c r="P8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>62</v>
-      </c>
-      <c r="S8" t="s">
-        <v>62</v>
-      </c>
-      <c r="T8" t="s">
-        <v>56</v>
-      </c>
-      <c r="U8" t="s">
-        <v>62</v>
-      </c>
-      <c r="W8" t="s">
-        <v>58</v>
-      </c>
-      <c r="X8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>58</v>
-      </c>
-      <c r="T9" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-      <c r="P10" t="s">
-        <v>53</v>
-      </c>
-      <c r="T10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="5:20" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1666,57 +1624,55 @@
     <row r="134" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O42"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A3:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="24" max="24" width="25.28515625" customWidth="1"/>
-    <col min="26" max="26" width="20.5703125" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" customWidth="1"/>
-    <col min="28" max="28" width="12.140625" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" customWidth="1"/>
-    <col min="30" max="30" width="13" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" customWidth="1"/>
-    <col min="42" max="42" width="11.42578125" customWidth="1"/>
-    <col min="49" max="49" width="16.85546875" customWidth="1"/>
-    <col min="50" max="50" width="13.28515625" customWidth="1"/>
-    <col min="54" max="54" width="15" customWidth="1"/>
-    <col min="62" max="62" width="11.7109375" customWidth="1"/>
-    <col min="86" max="86" width="15.28515625" customWidth="1"/>
-    <col min="87" max="87" width="33.85546875" customWidth="1"/>
-    <col min="93" max="93" width="14.28515625" customWidth="1"/>
-    <col min="94" max="94" width="15.28515625" customWidth="1"/>
-    <col min="100" max="100" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="22" max="22" width="25.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" customWidth="1"/>
+    <col min="28" max="28" width="13" customWidth="1"/>
+    <col min="32" max="32" width="11.5703125" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="13.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" customWidth="1"/>
+    <col min="47" max="47" width="16.85546875" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" customWidth="1"/>
+    <col min="52" max="52" width="15" customWidth="1"/>
+    <col min="60" max="60" width="11.7109375" customWidth="1"/>
+    <col min="84" max="84" width="15.28515625" customWidth="1"/>
+    <col min="85" max="85" width="33.85546875" customWidth="1"/>
+    <col min="91" max="91" width="14.28515625" customWidth="1"/>
+    <col min="92" max="92" width="15.28515625" customWidth="1"/>
+    <col min="98" max="98" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>48</v>
       </c>
       <c r="C3" t="s">
@@ -1729,715 +1685,683 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>59</v>
       </c>
       <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="I5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>40</v>
       </c>
       <c r="M5" t="s">
         <v>39</v>
       </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
         <v>33</v>
       </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" t="s">
-        <v>33</v>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" t="s">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" t="s">
-        <v>4</v>
-      </c>
-      <c r="O9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
       </c>
       <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" t="s">
-        <v>27</v>
-      </c>
       <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="L10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="N10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
+      <c r="F11" t="s">
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="I11" t="s">
-        <v>28</v>
-      </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N11" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" t="s">
         <v>32</v>
+      </c>
+      <c r="K12" t="s">
+        <v>0</v>
       </c>
       <c r="M12" t="s">
         <v>0</v>
       </c>
-      <c r="O12" t="s">
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
         <v>0</v>
       </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" t="s">
-        <v>12</v>
+      <c r="M17" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" t="s">
-        <v>7</v>
-      </c>
-      <c r="O15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M16" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" t="s">
-        <v>30</v>
-      </c>
       <c r="J18" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" t="s">
         <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
       </c>
       <c r="M18" t="s">
         <v>37</v>
       </c>
-      <c r="O18" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
         <v>7</v>
       </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
         <v>3</v>
       </c>
-      <c r="L19" t="s">
-        <v>3</v>
+      <c r="K19" t="s">
+        <v>24</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" t="s">
         <v>35</v>
       </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
       <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" t="s">
         <v>35</v>
       </c>
-      <c r="M20" t="s">
+      <c r="K20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
         <v>25</v>
       </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
       <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
         <v>19</v>
       </c>
-      <c r="M21" t="s">
+      <c r="K21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
-      <c r="G22" t="s">
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" t="s">
         <v>37</v>
       </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" t="s">
-        <v>13</v>
-      </c>
-      <c r="M22" t="s">
-        <v>31</v>
+      <c r="H27" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" spans="3:10" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2453,102 +2377,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O1898"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A3:M1898"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="96" zoomScaleNormal="130"/>
+    <sheetView zoomScale="96" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60" style="1" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="60.5703125" customWidth="1"/>
-    <col min="9" max="9" width="62.5703125" customWidth="1"/>
-    <col min="10" max="10" width="79.42578125" customWidth="1"/>
-    <col min="11" max="11" width="74" customWidth="1"/>
-    <col min="12" max="12" width="80.140625" customWidth="1"/>
-    <col min="13" max="13" width="56.42578125" customWidth="1"/>
-    <col min="14" max="14" width="53.7109375" customWidth="1"/>
-    <col min="15" max="15" width="58.28515625" customWidth="1"/>
-    <col min="16" max="16" width="57.42578125" customWidth="1"/>
-    <col min="17" max="17" width="59.7109375" customWidth="1"/>
-    <col min="18" max="18" width="73.85546875" customWidth="1"/>
-    <col min="19" max="19" width="53.42578125" customWidth="1"/>
-    <col min="20" max="20" width="70.28515625" customWidth="1"/>
-    <col min="21" max="21" width="42.28515625" customWidth="1"/>
-    <col min="22" max="22" width="71" customWidth="1"/>
-    <col min="23" max="23" width="68.28515625" customWidth="1"/>
-    <col min="24" max="24" width="62.42578125" customWidth="1"/>
-    <col min="25" max="25" width="55.5703125" customWidth="1"/>
-    <col min="26" max="26" width="64.5703125" customWidth="1"/>
-    <col min="27" max="27" width="48.42578125" customWidth="1"/>
-    <col min="28" max="28" width="78.85546875" customWidth="1"/>
-    <col min="29" max="29" width="69.42578125" customWidth="1"/>
-    <col min="30" max="30" width="68.85546875" customWidth="1"/>
-    <col min="31" max="31" width="66.28515625" customWidth="1"/>
-    <col min="32" max="32" width="82.85546875" customWidth="1"/>
-    <col min="33" max="33" width="53.140625" customWidth="1"/>
-    <col min="34" max="34" width="51.28515625" customWidth="1"/>
-    <col min="35" max="35" width="57.42578125" customWidth="1"/>
-    <col min="36" max="36" width="55.140625" customWidth="1"/>
-    <col min="37" max="37" width="46.7109375" customWidth="1"/>
-    <col min="38" max="38" width="48.140625" customWidth="1"/>
-    <col min="39" max="39" width="56.140625" customWidth="1"/>
-    <col min="40" max="40" width="48.5703125" customWidth="1"/>
-    <col min="41" max="41" width="40.28515625" customWidth="1"/>
-    <col min="42" max="42" width="65.28515625" customWidth="1"/>
-    <col min="43" max="43" width="71.85546875" customWidth="1"/>
-    <col min="44" max="44" width="62.7109375" customWidth="1"/>
-    <col min="45" max="45" width="53.28515625" customWidth="1"/>
-    <col min="46" max="46" width="58.140625" customWidth="1"/>
-    <col min="47" max="47" width="46.7109375" customWidth="1"/>
-    <col min="48" max="48" width="7.140625" customWidth="1"/>
-    <col min="49" max="49" width="57.85546875" customWidth="1"/>
-    <col min="50" max="50" width="60.7109375" customWidth="1"/>
-    <col min="51" max="51" width="52.28515625" customWidth="1"/>
-    <col min="52" max="52" width="75.7109375" customWidth="1"/>
-    <col min="53" max="53" width="45" customWidth="1"/>
-    <col min="54" max="54" width="69.140625" customWidth="1"/>
-    <col min="55" max="55" width="64.5703125" customWidth="1"/>
-    <col min="57" max="57" width="34.85546875" customWidth="1"/>
-    <col min="58" max="58" width="66.42578125" customWidth="1"/>
-    <col min="59" max="59" width="56" customWidth="1"/>
-    <col min="60" max="60" width="51.42578125" customWidth="1"/>
-    <col min="61" max="61" width="52.7109375" customWidth="1"/>
-    <col min="62" max="62" width="38.5703125" customWidth="1"/>
-    <col min="63" max="63" width="53.42578125" customWidth="1"/>
-    <col min="64" max="64" width="41" customWidth="1"/>
-    <col min="81" max="81" width="12.28515625" customWidth="1"/>
-    <col min="83" max="83" width="29.28515625" customWidth="1"/>
-    <col min="84" max="84" width="11.7109375" customWidth="1"/>
-    <col min="85" max="85" width="30.7109375" customWidth="1"/>
-    <col min="86" max="86" width="56.85546875" customWidth="1"/>
-    <col min="87" max="87" width="61.7109375" customWidth="1"/>
-    <col min="88" max="88" width="50" customWidth="1"/>
-    <col min="89" max="89" width="49.5703125" customWidth="1"/>
-    <col min="90" max="90" width="84.42578125" customWidth="1"/>
-    <col min="91" max="92" width="59.140625" customWidth="1"/>
-    <col min="93" max="93" width="68.140625" customWidth="1"/>
-    <col min="94" max="94" width="56.28515625" customWidth="1"/>
-    <col min="95" max="95" width="60" customWidth="1"/>
-    <col min="96" max="96" width="61" customWidth="1"/>
-    <col min="97" max="97" width="52.28515625" customWidth="1"/>
-    <col min="98" max="98" width="100" customWidth="1"/>
-    <col min="99" max="99" width="8.85546875" customWidth="1"/>
-    <col min="100" max="100" width="18.42578125" customWidth="1"/>
-    <col min="101" max="101" width="47.7109375" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" customWidth="1"/>
+    <col min="7" max="7" width="62.5703125" customWidth="1"/>
+    <col min="8" max="8" width="79.42578125" customWidth="1"/>
+    <col min="9" max="9" width="74" customWidth="1"/>
+    <col min="10" max="10" width="80.140625" customWidth="1"/>
+    <col min="11" max="11" width="56.42578125" customWidth="1"/>
+    <col min="12" max="12" width="53.7109375" customWidth="1"/>
+    <col min="13" max="13" width="58.28515625" customWidth="1"/>
+    <col min="14" max="14" width="57.42578125" customWidth="1"/>
+    <col min="15" max="15" width="59.7109375" customWidth="1"/>
+    <col min="16" max="16" width="73.85546875" customWidth="1"/>
+    <col min="17" max="17" width="53.42578125" customWidth="1"/>
+    <col min="18" max="18" width="70.28515625" customWidth="1"/>
+    <col min="19" max="19" width="42.28515625" customWidth="1"/>
+    <col min="20" max="20" width="71" customWidth="1"/>
+    <col min="21" max="21" width="68.28515625" customWidth="1"/>
+    <col min="22" max="22" width="62.42578125" customWidth="1"/>
+    <col min="23" max="23" width="55.5703125" customWidth="1"/>
+    <col min="24" max="24" width="64.5703125" customWidth="1"/>
+    <col min="25" max="25" width="48.42578125" customWidth="1"/>
+    <col min="26" max="26" width="78.85546875" customWidth="1"/>
+    <col min="27" max="27" width="69.42578125" customWidth="1"/>
+    <col min="28" max="28" width="68.85546875" customWidth="1"/>
+    <col min="29" max="29" width="66.28515625" customWidth="1"/>
+    <col min="30" max="30" width="82.85546875" customWidth="1"/>
+    <col min="31" max="31" width="53.140625" customWidth="1"/>
+    <col min="32" max="32" width="51.28515625" customWidth="1"/>
+    <col min="33" max="33" width="57.42578125" customWidth="1"/>
+    <col min="34" max="34" width="55.140625" customWidth="1"/>
+    <col min="35" max="35" width="46.7109375" customWidth="1"/>
+    <col min="36" max="36" width="48.140625" customWidth="1"/>
+    <col min="37" max="37" width="56.140625" customWidth="1"/>
+    <col min="38" max="38" width="48.5703125" customWidth="1"/>
+    <col min="39" max="39" width="40.28515625" customWidth="1"/>
+    <col min="40" max="40" width="65.28515625" customWidth="1"/>
+    <col min="41" max="41" width="71.85546875" customWidth="1"/>
+    <col min="42" max="42" width="62.7109375" customWidth="1"/>
+    <col min="43" max="43" width="53.28515625" customWidth="1"/>
+    <col min="44" max="44" width="58.140625" customWidth="1"/>
+    <col min="45" max="45" width="46.7109375" customWidth="1"/>
+    <col min="46" max="46" width="7.140625" customWidth="1"/>
+    <col min="47" max="47" width="57.85546875" customWidth="1"/>
+    <col min="48" max="48" width="60.7109375" customWidth="1"/>
+    <col min="49" max="49" width="52.28515625" customWidth="1"/>
+    <col min="50" max="50" width="75.7109375" customWidth="1"/>
+    <col min="51" max="51" width="45" customWidth="1"/>
+    <col min="52" max="52" width="69.140625" customWidth="1"/>
+    <col min="53" max="53" width="64.5703125" customWidth="1"/>
+    <col min="55" max="55" width="34.85546875" customWidth="1"/>
+    <col min="56" max="56" width="66.42578125" customWidth="1"/>
+    <col min="57" max="57" width="56" customWidth="1"/>
+    <col min="58" max="58" width="51.42578125" customWidth="1"/>
+    <col min="59" max="59" width="52.7109375" customWidth="1"/>
+    <col min="60" max="60" width="38.5703125" customWidth="1"/>
+    <col min="61" max="61" width="53.42578125" customWidth="1"/>
+    <col min="62" max="62" width="41" customWidth="1"/>
+    <col min="79" max="79" width="12.28515625" customWidth="1"/>
+    <col min="81" max="81" width="29.28515625" customWidth="1"/>
+    <col min="82" max="82" width="11.7109375" customWidth="1"/>
+    <col min="83" max="83" width="30.7109375" customWidth="1"/>
+    <col min="84" max="84" width="56.85546875" customWidth="1"/>
+    <col min="85" max="85" width="61.7109375" customWidth="1"/>
+    <col min="86" max="86" width="50" customWidth="1"/>
+    <col min="87" max="87" width="49.5703125" customWidth="1"/>
+    <col min="88" max="88" width="84.42578125" customWidth="1"/>
+    <col min="89" max="90" width="59.140625" customWidth="1"/>
+    <col min="91" max="91" width="68.140625" customWidth="1"/>
+    <col min="92" max="92" width="56.28515625" customWidth="1"/>
+    <col min="93" max="93" width="60" customWidth="1"/>
+    <col min="94" max="94" width="61" customWidth="1"/>
+    <col min="95" max="95" width="52.28515625" customWidth="1"/>
+    <col min="96" max="96" width="100" customWidth="1"/>
+    <col min="97" max="97" width="8.85546875" customWidth="1"/>
+    <col min="98" max="98" width="18.42578125" customWidth="1"/>
+    <col min="99" max="99" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>48</v>
       </c>
       <c r="C3" t="s">
@@ -2561,213 +2485,199 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>59</v>
       </c>
       <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="L3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="N3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" t="s">
-        <v>58</v>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L4" t="s">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>74</v>
       </c>
-      <c r="M4" t="s">
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="N4" t="s">
+      <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="O4" t="s">
+      <c r="F5" t="s">
         <v>77</v>
       </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" t="s">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="M5" t="s">
+      <c r="C6" t="s">
         <v>85</v>
       </c>
-      <c r="N5" t="s">
+      <c r="E6" t="s">
         <v>86</v>
       </c>
-      <c r="O5" t="s">
+      <c r="F6" t="s">
         <v>87</v>
       </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" t="s">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="L6" t="s">
+      <c r="C7" t="s">
         <v>94</v>
       </c>
-      <c r="M6" t="s">
+      <c r="E7" t="s">
         <v>95</v>
       </c>
-      <c r="O6" t="s">
+      <c r="F7" t="s">
         <v>96</v>
       </c>
+      <c r="H7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" t="s">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>101</v>
       </c>
-      <c r="L7" t="s">
+      <c r="C8" t="s">
         <v>102</v>
       </c>
-      <c r="M7" t="s">
+      <c r="E8" t="s">
         <v>103</v>
       </c>
-      <c r="O7" t="s">
+      <c r="F8" t="s">
         <v>104</v>
       </c>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" t="s">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>107</v>
       </c>
-      <c r="H8" t="s">
+      <c r="E9" t="s">
         <v>108</v>
       </c>
-      <c r="J8" t="s">
+      <c r="F9" t="s">
         <v>109</v>
       </c>
-      <c r="M8" t="s">
+      <c r="H9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="3:10" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4652,6 +4562,6 @@
     <row r="1898" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>